<commit_message>
Atualização automática de TUPANCIRETA.xlsx
</commit_message>
<xml_diff>
--- a/TUPANCIRETA.xlsx
+++ b/TUPANCIRETA.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CACAA65-FF8E-4260-8D38-D0ADEEC54581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{007916A8-D629-4518-9C32-CB91B6548BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="6" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="7" r:id="rId1"/>
     <sheet name="DESFAZIMENTOS" sheetId="1" r:id="rId2"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="2" r:id="rId3"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="3" r:id="rId4"/>
     <sheet name="CPIP" sheetId="4" r:id="rId5"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
+    <sheet name="DGC" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="305">
   <si>
     <t>COMARCA</t>
   </si>
@@ -928,6 +929,18 @@
   </si>
   <si>
     <t>Não finalizou procedimentos de eliminação</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MAOBRAS/MATIC</t>
+  </si>
+  <si>
+    <t>Atraso no ateste. Off-line no Teams.</t>
   </si>
 </sst>
 </file>
@@ -937,7 +950,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,6 +1003,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1004,7 +1030,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1045,6 +1071,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
         <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1117,9 +1149,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1186,12 +1218,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{DB2162BF-39F4-40D1-8CD6-7A1DFDAD69DF}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4B351D58-DED1-4FC5-8C00-53235BCC7EC0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1221,10 +1257,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5726C52B-C02C-438E-A49F-731A77FA5975}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D86B9B9-6A9A-4856-A050-DC491A6B671E}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1262,7 +1298,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAF628D4-04F7-4170-B2AC-84651FD9773E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FED121-C795-4A47-8ADF-09520072F389}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1325,7 +1361,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F461AA25-D8A9-4B6F-BF00-35E16B759706}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55791394-930E-48C9-8990-7D67B5D29CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1344,7 +1380,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B2376C-8EA2-FC83-8EEC-6FEBDDC80228}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC749F1-3C52-FF5E-D963-B6CF2DC9D65D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1393,7 +1429,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EF03428-F57F-C646-5306-DD22D5050A11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{671F1FF2-6867-689C-E478-7BA5825C6818}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1412,7 +1448,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C9C1C44-6C13-DA74-1289-0678E7D60AAB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB256C74-5566-98AF-8DB5-6A904840D581}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1443,7 +1479,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{042A9E81-7B5E-3C1F-3C29-3539AC3FAD82}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B4D9840-1A18-97BA-93E3-5FF0D416BEFF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1474,7 +1510,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{668F9DB0-CB4D-5B3F-6259-CF050AD33A25}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF57400C-BB7F-C6EF-95EC-3F37348A188E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1517,7 +1553,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6FA97C-EFFE-4848-AEFF-3EED7F471DC7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A658B1C-3231-4ED9-B22B-961965336C2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1555,7 +1591,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D929082-FACB-4374-9179-0E40158F4CF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFC98E04-46C6-47C9-B44A-63D168EBF33D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1598,7 +1634,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C114B289-010D-46CF-ABBF-773FF9040ED2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE293069-1573-4D8E-8BA4-4081C2889A90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1911,7 +1947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC6E268-5C63-4028-8B36-B154E02A5D14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CCE249-6A81-4361-B28F-1F2407FD5492}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1923,98 +1959,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="29"/>
-    <col min="6" max="6" width="2" style="29" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="29" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="29"/>
+    <col min="1" max="5" width="12.5703125" style="31"/>
+    <col min="6" max="6" width="2" style="31" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="31" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="28"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="28"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="28"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="28"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="28"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="28"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="28"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="28"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="28"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="28"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="28"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="28"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="28"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="28"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="28"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="28"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="28"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="28"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="28"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="28"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="28"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="28"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="28"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="28"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="28"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="28"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="28"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="28"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="28"/>
+      <c r="F29" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5475,4 +5511,44 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>